<commit_message>
Created Notebook-Validation to validate prediction models.
</commit_message>
<xml_diff>
--- a/reports/Timeseries vs Regression Prediction.xlsx
+++ b/reports/Timeseries vs Regression Prediction.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koonleong/Documents/UM/UMMADS/Courses - Current/SIADS697-Capstone/power_emissions/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FE2071D-4CD5-B741-9CA8-BACA2EB84AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678515C5-A819-B742-8B01-96F8F830A22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="560" windowWidth="33480" windowHeight="20380" xr2:uid="{AB0DD39C-58FC-8A4E-82AA-A499FF20AFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
   <si>
     <t>Cluster 0</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Growth</t>
   </si>
   <si>
-    <t>Raw</t>
-  </si>
-  <si>
     <t>Difference between Regression Model and Timeseries</t>
   </si>
   <si>
@@ -64,6 +61,21 @@
   </si>
   <si>
     <t>Clustered vs Global Predictions</t>
+  </si>
+  <si>
+    <t>Timeseries</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>TS vs Panel</t>
+  </si>
+  <si>
+    <t>Regression vs Panel</t>
   </si>
 </sst>
 </file>
@@ -115,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -135,11 +147,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -456,22 +472,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30AE331-8568-774C-8853-F571EAA584D8}">
-  <dimension ref="A2:I57"/>
+  <dimension ref="A2:V55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="7" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="26.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="4.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="5"/>
+    <col min="16" max="16" width="7.5" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -485,15 +506,50 @@
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2021</v>
       </c>
@@ -510,15 +566,15 @@
         <f>SUM(B3:D3)</f>
         <v>34315.913080999999</v>
       </c>
-      <c r="G3" s="2">
+      <c r="F3" s="2">
         <v>33724.671875</v>
       </c>
-      <c r="I3" s="8">
-        <f>(E3/G3)-1</f>
+      <c r="H3" s="7">
+        <f>(E3/F3)-1</f>
         <v>1.7531414632925957E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2022</v>
       </c>
@@ -535,15 +591,15 @@
         <f t="shared" ref="E4:E7" si="0">SUM(B4:D4)</f>
         <v>34444.188700999999</v>
       </c>
-      <c r="G4" s="2">
+      <c r="F4" s="2">
         <v>34152.289062000003</v>
       </c>
-      <c r="I4" s="8">
-        <f t="shared" ref="I4:I7" si="1">(E4/G4)-1</f>
+      <c r="H4" s="7">
+        <f>(E4/F4)-1</f>
         <v>8.5470007140686644E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2023</v>
       </c>
@@ -560,15 +616,15 @@
         <f t="shared" si="0"/>
         <v>34497.505782</v>
       </c>
-      <c r="G5" s="2">
+      <c r="F5" s="2">
         <v>34579.898437999997</v>
       </c>
-      <c r="I5" s="8">
-        <f t="shared" si="1"/>
+      <c r="H5" s="7">
+        <f>(E5/F5)-1</f>
         <v>-2.3826748984737689E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>2024</v>
       </c>
@@ -585,15 +641,15 @@
         <f t="shared" si="0"/>
         <v>34721.234599000003</v>
       </c>
-      <c r="G6" s="2">
+      <c r="F6" s="2">
         <v>35007.507812000003</v>
       </c>
-      <c r="I6" s="8">
-        <f t="shared" si="1"/>
+      <c r="H6" s="7">
+        <f>(E6/F6)-1</f>
         <v>-8.1774805146760388E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2025</v>
       </c>
@@ -610,30 +666,71 @@
         <f t="shared" si="0"/>
         <v>34849.506318</v>
       </c>
-      <c r="G7" s="2">
+      <c r="F7" s="2">
         <v>35435.125</v>
       </c>
-      <c r="I7" s="8">
+      <c r="H7" s="7">
+        <f>(E7/F7)-1</f>
+        <v>-1.6526502502813289E-2</v>
+      </c>
+      <c r="J7" s="5">
+        <v>2025</v>
+      </c>
+      <c r="K7" s="2">
+        <v>784</v>
+      </c>
+      <c r="L7" s="2">
+        <v>19664</v>
+      </c>
+      <c r="M7" s="2">
+        <v>16943</v>
+      </c>
+      <c r="N7" s="2">
+        <v>37391</v>
+      </c>
+      <c r="O7" s="2">
+        <v>40604</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>2025</v>
+      </c>
+      <c r="R7" s="8">
+        <f>(K7/B7)-1</f>
+        <v>-0.49474211534775725</v>
+      </c>
+      <c r="S7" s="8">
+        <f t="shared" ref="S7:V7" si="1">(L7/C7)-1</f>
+        <v>0.28765330844147385</v>
+      </c>
+      <c r="T7" s="8">
         <f t="shared" si="1"/>
-        <v>-1.6526502502813289E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-6.0112845733033771E-2</v>
+      </c>
+      <c r="U7" s="8">
+        <f t="shared" si="1"/>
+        <v>7.2927681064087313E-2</v>
+      </c>
+      <c r="V7" s="8">
+        <f t="shared" si="1"/>
+        <v>0.14586868255720842</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -649,12 +746,11 @@
       <c r="E24" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>2021</v>
       </c>
@@ -674,12 +770,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G25" s="2">
-        <f t="shared" ref="G25" si="3">G3/G$3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F25" s="2">
+        <f t="shared" ref="F25" si="3">F3/F$3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>2022</v>
       </c>
@@ -699,12 +795,12 @@
         <f t="shared" si="4"/>
         <v>1.0037380797560949</v>
       </c>
-      <c r="G26" s="2">
-        <f t="shared" ref="G26" si="5">G4/G$3</f>
+      <c r="F26" s="2">
+        <f t="shared" ref="F26" si="5">F4/F$3</f>
         <v>1.0126796544851484</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>2023</v>
       </c>
@@ -724,12 +820,12 @@
         <f t="shared" si="4"/>
         <v>1.0052917927776355</v>
       </c>
-      <c r="G27" s="2">
-        <f t="shared" ref="G27" si="6">G5/G$3</f>
+      <c r="F27" s="2">
+        <f t="shared" ref="F27" si="6">F5/F$3</f>
         <v>1.0253590773594441</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>2024</v>
       </c>
@@ -749,12 +845,12 @@
         <f t="shared" si="4"/>
         <v>1.0118114740832709</v>
       </c>
-      <c r="G28" s="2">
-        <f t="shared" ref="G28" si="7">G6/G$3</f>
+      <c r="F28" s="2">
+        <f t="shared" ref="F28" si="7">F6/F$3</f>
         <v>1.0380385001744366</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>2025</v>
       </c>
@@ -774,488 +870,554 @@
         <f t="shared" si="4"/>
         <v>1.0155494401603273</v>
       </c>
-      <c r="G29" s="2">
-        <f t="shared" ref="G29" si="8">G7/G$3</f>
+      <c r="F29" s="2">
+        <f t="shared" ref="F29" si="8">F7/F$3</f>
         <v>1.0507181546892368</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="5" t="s">
+    <row r="32" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="C32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I34" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H32" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V32" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>2021</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1440.334014</v>
+      </c>
+      <c r="C33" s="2">
+        <v>15584.938375</v>
+      </c>
+      <c r="D33" s="2">
+        <v>16736.470646999998</v>
+      </c>
+      <c r="E33" s="2">
+        <f>SUM(B33:D33)</f>
+        <v>33761.743036</v>
+      </c>
+      <c r="F33" s="2">
+        <v>33649.523963</v>
+      </c>
+      <c r="H33" s="7">
+        <f>(E33/F33)-1</f>
+        <v>3.3349379065032991E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>2022</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1461.9160280000001</v>
+      </c>
+      <c r="C34" s="2">
+        <v>15757.940095</v>
+      </c>
+      <c r="D34" s="2">
+        <v>16643.829624000002</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" ref="E34:E37" si="9">SUM(B34:D34)</f>
+        <v>33863.685747000003</v>
+      </c>
+      <c r="F34" s="2">
+        <v>33946.976429000002</v>
+      </c>
+      <c r="H34" s="7">
+        <f>(E34/F34)-1</f>
+        <v>-2.4535522971891321E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B35" s="2">
-        <v>1440.334014</v>
+        <v>1483.4980410000001</v>
       </c>
       <c r="C35" s="2">
-        <v>15584.938375</v>
+        <v>15674.716973000001</v>
       </c>
       <c r="D35" s="2">
-        <v>16736.470646999998</v>
+        <v>16578.092111000002</v>
       </c>
       <c r="E35" s="2">
-        <f>SUM(B35:D35)</f>
-        <v>33761.743036</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2">
-        <v>33649.523963</v>
-      </c>
-      <c r="I35" s="8">
-        <f>(E35/G35)-1</f>
-        <v>3.3349379065032991E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>33736.307125000007</v>
+      </c>
+      <c r="F35" s="2">
+        <v>33823.943887000001</v>
+      </c>
+      <c r="H35" s="7">
+        <f>(E35/F35)-1</f>
+        <v>-2.590968170145258E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="B36" s="2">
-        <v>1461.9160280000001</v>
+        <v>1505.0800549999999</v>
       </c>
       <c r="C36" s="2">
-        <v>15757.940095</v>
+        <v>15914.347406999999</v>
       </c>
       <c r="D36" s="2">
-        <v>16643.829624000002</v>
+        <v>16516.861879</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" ref="E36:E39" si="9">SUM(B36:D36)</f>
-        <v>33863.685747000003</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <v>33946.976429000002</v>
-      </c>
-      <c r="I36" s="8">
-        <f t="shared" ref="I36:I39" si="10">(E36/G36)-1</f>
-        <v>-2.4535522971891321E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>33936.289340999996</v>
+      </c>
+      <c r="F36" s="2">
+        <v>33850.035673999999</v>
+      </c>
+      <c r="H36" s="7">
+        <f>(E36/F36)-1</f>
+        <v>2.5481115538747989E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B37" s="2">
-        <v>1483.4980410000001</v>
+        <v>1526.662069</v>
       </c>
       <c r="C37" s="2">
-        <v>15674.716973000001</v>
+        <v>16318.29595</v>
       </c>
       <c r="D37" s="2">
-        <v>16578.092111000002</v>
+        <v>16456.386775999999</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="9"/>
-        <v>33736.307125000007</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <v>33823.943887000001</v>
-      </c>
-      <c r="I37" s="8">
-        <f t="shared" si="10"/>
-        <v>-2.590968170145258E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+        <v>34301.344794999997</v>
+      </c>
+      <c r="F37" s="2">
+        <v>34459.793766000003</v>
+      </c>
+      <c r="H37" s="7">
+        <f>(E37/F37)-1</f>
+        <v>-4.598082393526659E-3</v>
+      </c>
+      <c r="J37" s="5">
+        <v>2025</v>
+      </c>
+      <c r="K37" s="2">
+        <v>784</v>
+      </c>
+      <c r="L37" s="2">
+        <v>19664</v>
+      </c>
+      <c r="M37" s="2">
+        <v>16943</v>
+      </c>
+      <c r="N37" s="2">
+        <v>37391</v>
+      </c>
+      <c r="O37" s="2">
+        <v>40604</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>2025</v>
+      </c>
+      <c r="R37" s="8">
+        <f>(K37/B37)-1</f>
+        <v>-0.48646133553738014</v>
+      </c>
+      <c r="S37" s="8">
+        <f t="shared" ref="S37" si="10">(L37/C37)-1</f>
+        <v>0.20502778355358853</v>
+      </c>
+      <c r="T37" s="8">
+        <f t="shared" ref="T37" si="11">(M37/D37)-1</f>
+        <v>2.9569870386716879E-2</v>
+      </c>
+      <c r="U37" s="8">
+        <f t="shared" ref="U37" si="12">(N37/E37)-1</f>
+        <v>9.0073879711281002E-2</v>
+      </c>
+      <c r="V37" s="8">
+        <f t="shared" ref="V37" si="13">(O37/F37)-1</f>
+        <v>0.17830072564340838</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>2021</v>
+      </c>
+      <c r="B40" s="2">
+        <f>B33/B$33</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" ref="C40:E40" si="14">C33/C$33</f>
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" ref="F40" si="15">F33/F$33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>2022</v>
+      </c>
+      <c r="B41" s="2">
+        <f t="shared" ref="B41:E44" si="16">B34/B$33</f>
+        <v>1.0149840341130762</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0111005713232408</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="16"/>
+        <v>0.9944647216875081</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0030194741690706</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" ref="F41" si="17">F34/F$33</f>
+        <v>1.0088397228539421</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>2023</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" si="16"/>
+        <v>1.029968067531869</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="16"/>
+        <v>1.005760600128135</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="16"/>
+        <v>0.99053692147284433</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="16"/>
+        <v>0.99924660551521671</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" ref="F42" si="18">F35/F$33</f>
+        <v>1.0051834291680259</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
         <v>2024</v>
       </c>
-      <c r="B38" s="2">
-        <v>1505.0800549999999</v>
-      </c>
-      <c r="C38" s="2">
-        <v>15914.347406999999</v>
-      </c>
-      <c r="D38" s="2">
-        <v>16516.861879</v>
-      </c>
-      <c r="E38" s="2">
-        <f t="shared" si="9"/>
-        <v>33936.289340999996</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2">
-        <v>33850.035673999999</v>
-      </c>
-      <c r="I38" s="8">
-        <f t="shared" si="10"/>
-        <v>2.5481115538747989E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+      <c r="B43" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0449521016449452</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0211363705183722</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="16"/>
+        <v>0.98687843018806576</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0051699435308739</v>
+      </c>
+      <c r="F43" s="2">
+        <f t="shared" ref="F43" si="19">F36/F$33</f>
+        <v>1.0059588275667875</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
         <v>2025</v>
       </c>
-      <c r="B39" s="2">
-        <v>1526.662069</v>
-      </c>
-      <c r="C39" s="2">
-        <v>16318.29595</v>
-      </c>
-      <c r="D39" s="2">
-        <v>16456.386775999999</v>
-      </c>
-      <c r="E39" s="2">
-        <f t="shared" si="9"/>
-        <v>34301.344794999997</v>
-      </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2">
-        <v>34459.793766000003</v>
-      </c>
-      <c r="I39" s="8">
-        <f t="shared" si="10"/>
-        <v>-4.598082393526659E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="B44" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0599361357580215</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0470555325503492</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="16"/>
+        <v>0.98326505767509564</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0159826392382829</v>
+      </c>
+      <c r="F44" s="2">
+        <f t="shared" ref="F44" si="20">F37/F$33</f>
+        <v>1.0240796810050254</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="J48" s="4"/>
+      <c r="Q48" s="4"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="J49" s="4"/>
+      <c r="Q49" s="4"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="C50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5" t="s">
+      <c r="F50" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
         <v>2021</v>
       </c>
-      <c r="B42" s="2">
-        <f>B35/B$35</f>
-        <v>1</v>
-      </c>
-      <c r="C42" s="2">
-        <f t="shared" ref="C42:E42" si="11">C35/C$35</f>
-        <v>1</v>
-      </c>
-      <c r="D42" s="2">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="2">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="G42" s="2">
-        <f t="shared" ref="G42" si="12">G35/G$35</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
+      <c r="B51" s="3">
+        <f>(B33/B3)-1</f>
+        <v>2.3239773334021718E-2</v>
+      </c>
+      <c r="C51" s="3">
+        <f>(C33/C3)-1</f>
+        <v>2.0287868082388139E-2</v>
+      </c>
+      <c r="D51" s="3">
+        <f>(D33/D3)-1</f>
+        <v>-5.0857372918723831E-2</v>
+      </c>
+      <c r="E51" s="3">
+        <f>(E33/E3)-1</f>
+        <v>-1.6149068908407727E-2</v>
+      </c>
+      <c r="F51" s="3">
+        <f>(F33/F3)-1</f>
+        <v>-2.2282770393893259E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
         <v>2022</v>
       </c>
-      <c r="B43" s="2">
-        <f t="shared" ref="B43:E46" si="13">B36/B$35</f>
-        <v>1.0149840341130762</v>
-      </c>
-      <c r="C43" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0111005713232408</v>
-      </c>
-      <c r="D43" s="2">
-        <f t="shared" si="13"/>
-        <v>0.9944647216875081</v>
-      </c>
-      <c r="E43" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0030194741690706</v>
-      </c>
-      <c r="G43" s="2">
-        <f t="shared" ref="G43" si="14">G36/G$35</f>
-        <v>1.0088397228539421</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
+      <c r="B52" s="3">
+        <f>(B34/B4)-1</f>
+        <v>1.2661986744602949E-2</v>
+      </c>
+      <c r="C52" s="3">
+        <f>(C34/C4)-1</f>
+        <v>3.1613646332274037E-2</v>
+      </c>
+      <c r="D52" s="3">
+        <f>(D34/D4)-1</f>
+        <v>-6.1024020673611234E-2</v>
+      </c>
+      <c r="E52" s="3">
+        <f>(E34/E4)-1</f>
+        <v>-1.6853436701301683E-2</v>
+      </c>
+      <c r="F52" s="3">
+        <f>(F34/F4)-1</f>
+        <v>-6.0116799968306101E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
         <v>2023</v>
       </c>
-      <c r="B44" s="2">
-        <f t="shared" si="13"/>
-        <v>1.029968067531869</v>
-      </c>
-      <c r="C44" s="2">
-        <f t="shared" si="13"/>
-        <v>1.005760600128135</v>
-      </c>
-      <c r="D44" s="2">
-        <f t="shared" si="13"/>
-        <v>0.99053692147284433</v>
-      </c>
-      <c r="E44" s="2">
-        <f t="shared" si="13"/>
-        <v>0.99924660551521671</v>
-      </c>
-      <c r="G44" s="2">
-        <f t="shared" ref="G44" si="15">G37/G$35</f>
-        <v>1.0051834291680259</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
+      <c r="B53" s="3">
+        <f>(B35/B5)-1</f>
+        <v>2.5992197760540403E-3</v>
+      </c>
+      <c r="C53" s="3">
+        <f>(C35/C5)-1</f>
+        <v>3.5194106520053614E-2</v>
+      </c>
+      <c r="D53" s="3">
+        <f>(D35/D5)-1</f>
+        <v>-7.2608210387303473E-2</v>
+      </c>
+      <c r="E53" s="3">
+        <f>(E35/E5)-1</f>
+        <v>-2.2065324426937871E-2</v>
+      </c>
+      <c r="F53" s="3">
+        <f>(F35/F5)-1</f>
+        <v>-2.1861098069891227E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
         <v>2024</v>
       </c>
-      <c r="B45" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0449521016449452</v>
-      </c>
-      <c r="C45" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0211363705183722</v>
-      </c>
-      <c r="D45" s="2">
-        <f t="shared" si="13"/>
-        <v>0.98687843018806576</v>
-      </c>
-      <c r="E45" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0051699435308739</v>
-      </c>
-      <c r="G45" s="2">
-        <f t="shared" ref="G45" si="16">G38/G$35</f>
-        <v>1.0059588275667875</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
+      <c r="B54" s="3">
+        <f>(B36/B6)-1</f>
+        <v>-6.9853217408875068E-3</v>
+      </c>
+      <c r="C54" s="3">
+        <f>(C36/C6)-1</f>
+        <v>4.21156473917077E-2</v>
+      </c>
+      <c r="D54" s="3">
+        <f>(D36/D6)-1</f>
+        <v>-7.9038933678373224E-2</v>
+      </c>
+      <c r="E54" s="3">
+        <f>(E36/E6)-1</f>
+        <v>-2.2607066455598179E-2</v>
+      </c>
+      <c r="F54" s="3">
+        <f>(F36/F6)-1</f>
+        <v>-3.3063540090198629E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
         <v>2025</v>
       </c>
-      <c r="B46" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0599361357580215</v>
-      </c>
-      <c r="C46" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0470555325503492</v>
-      </c>
-      <c r="D46" s="2">
-        <f t="shared" si="13"/>
-        <v>0.98326505767509564</v>
-      </c>
-      <c r="E46" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0159826392382829</v>
-      </c>
-      <c r="G46" s="2">
-        <f t="shared" ref="G46" si="17">G39/G$35</f>
-        <v>1.0240796810050254</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="5">
-        <v>2021</v>
-      </c>
-      <c r="B53" s="3">
-        <f>(B35/B3)-1</f>
-        <v>2.3239773334021718E-2</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" ref="C53:E53" si="18">(C35/C3)-1</f>
-        <v>2.0287868082388139E-2</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="18"/>
-        <v>-5.0857372918723831E-2</v>
-      </c>
-      <c r="E53" s="3">
-        <f t="shared" si="18"/>
-        <v>-1.6149068908407727E-2</v>
-      </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3">
-        <f t="shared" ref="G53" si="19">(G35/G3)-1</f>
-        <v>-2.2282770393893259E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="5">
-        <v>2022</v>
-      </c>
-      <c r="B54" s="3">
-        <f t="shared" ref="B54:E54" si="20">(B36/B4)-1</f>
-        <v>1.2661986744602949E-2</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="20"/>
-        <v>3.1613646332274037E-2</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="20"/>
-        <v>-6.1024020673611234E-2</v>
-      </c>
-      <c r="E54" s="3">
-        <f t="shared" si="20"/>
-        <v>-1.6853436701301683E-2</v>
-      </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3">
-        <f t="shared" ref="G54" si="21">(G36/G4)-1</f>
-        <v>-6.0116799968306101E-3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="5">
-        <v>2023</v>
-      </c>
       <c r="B55" s="3">
-        <f t="shared" ref="B55:E55" si="22">(B37/B5)-1</f>
-        <v>2.5992197760540403E-3</v>
+        <f>(B37/B7)-1</f>
+        <v>-1.6124939334494659E-2</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" si="22"/>
-        <v>3.5194106520053614E-2</v>
+        <f>(C37/C7)-1</f>
+        <v>6.8567319372691449E-2</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" si="22"/>
-        <v>-7.2608210387303473E-2</v>
+        <f>(D37/D7)-1</f>
+        <v>-8.7106974183369323E-2</v>
       </c>
       <c r="E55" s="3">
-        <f t="shared" si="22"/>
-        <v>-2.2065324426937871E-2</v>
-      </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3">
-        <f t="shared" ref="G55" si="23">(G37/G5)-1</f>
-        <v>-2.1861098069891227E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="5">
-        <v>2024</v>
-      </c>
-      <c r="B56" s="3">
-        <f t="shared" ref="B56:E56" si="24">(B38/B6)-1</f>
-        <v>-6.9853217408875068E-3</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" si="24"/>
-        <v>4.21156473917077E-2</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="24"/>
-        <v>-7.9038933678373224E-2</v>
-      </c>
-      <c r="E56" s="3">
-        <f t="shared" si="24"/>
-        <v>-2.2607066455598179E-2</v>
-      </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3">
-        <f t="shared" ref="G56" si="25">(G38/G6)-1</f>
-        <v>-3.3063540090198629E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="5">
-        <v>2025</v>
-      </c>
-      <c r="B57" s="3">
-        <f t="shared" ref="B57:E57" si="26">(B39/B7)-1</f>
-        <v>-1.6124939334494659E-2</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" si="26"/>
-        <v>6.8567319372691449E-2</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="26"/>
-        <v>-8.7106974183369323E-2</v>
-      </c>
-      <c r="E57" s="3">
-        <f t="shared" si="26"/>
+        <f>(E37/E7)-1</f>
         <v>-1.5729391343396792E-2</v>
       </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3">
-        <f t="shared" ref="G57" si="27">(G39/G7)-1</f>
+      <c r="F55" s="3">
+        <f>(F37/F7)-1</f>
         <v>-2.7524419174477233E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E3:E7 E35:E39" formulaRange="1"/>
+    <ignoredError sqref="E3:E7 E33:E37" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>